<commit_message>
too many!! Don't know what to comment lol
</commit_message>
<xml_diff>
--- a/Data/Abney_data.xlsx
+++ b/Data/Abney_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pramodhegde/Documents/DSA/licor_2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAF2727-5B37-6F45-87E2-D5557F392F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134C2D1D-0CB1-7742-9CDA-A47054D2E04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1801"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A876" workbookViewId="0">
+      <selection activeCell="G901" sqref="G901"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21374,7 +21374,7 @@
         <v>6.3</v>
       </c>
       <c r="G881" s="1">
-        <v>4.3749999999999997E-2</v>
+        <v>0.54374999999999996</v>
       </c>
       <c r="H881">
         <v>5.8220000000000001</v>
@@ -21421,7 +21421,7 @@
         <v>6.3</v>
       </c>
       <c r="G883" s="1">
-        <v>4.4444444444444446E-2</v>
+        <v>0.5444444444444444</v>
       </c>
       <c r="H883">
         <v>5.77</v>
@@ -21468,7 +21468,7 @@
         <v>6</v>
       </c>
       <c r="G885" s="1">
-        <v>4.6527777777777779E-2</v>
+        <v>0.54652777777777772</v>
       </c>
       <c r="H885">
         <v>4.2869999999999999</v>
@@ -21515,7 +21515,7 @@
         <v>6</v>
       </c>
       <c r="G887" s="1">
-        <v>4.7222222222222221E-2</v>
+        <v>0.54722222222222228</v>
       </c>
       <c r="H887">
         <v>4.3449999999999998</v>
@@ -21562,7 +21562,7 @@
         <v>6</v>
       </c>
       <c r="G889" s="1">
-        <v>4.791666666666667E-2</v>
+        <v>0.54791666666666672</v>
       </c>
       <c r="H889">
         <v>4.1449999999999996</v>
@@ -21609,7 +21609,7 @@
         <v>7.6</v>
       </c>
       <c r="G891" s="1">
-        <v>5.486111111111111E-2</v>
+        <v>0.55486111111111114</v>
       </c>
       <c r="H891">
         <v>4.4909999999999997</v>
@@ -21738,7 +21738,7 @@
         <v>7.5</v>
       </c>
       <c r="G897" s="1">
-        <v>5.8333333333333334E-2</v>
+        <v>0.55833333333333335</v>
       </c>
       <c r="H897">
         <v>4.9429999999999996</v>
@@ -21785,7 +21785,7 @@
         <v>7.5</v>
       </c>
       <c r="G899" s="1">
-        <v>5.9722222222222225E-2</v>
+        <v>0.55972222222222223</v>
       </c>
       <c r="H899">
         <v>4.875</v>
@@ -21832,7 +21832,7 @@
         <v>7.5</v>
       </c>
       <c r="G901" s="1">
-        <v>6.0416666666666667E-2</v>
+        <v>0.56041666666666667</v>
       </c>
       <c r="H901">
         <v>4.5789999999999997</v>

</xml_diff>